<commit_message>
Fixed new defines with update 1.5.2 beta Fixed GER and SOV equipment errors caused by 1.5.2. Fixed paradox adding 1 prov
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="18180" windowHeight="8085" activeTab="2"/>
+    <workbookView xWindow="2100" yWindow="0" windowWidth="18180" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Skill level" sheetId="3" r:id="rId1"/>
@@ -355,11 +355,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$A$3" fmlaRange="Skills!$A$2:$A$10" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$A$3" fmlaRange="Skills!$A$2:$A$10" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$5" fmlaRange="Personality!$B$2:$B$25" noThreeD="1" sel="8" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$5" fmlaRange="Personality!$B$2:$B$25" noThreeD="1" sel="3" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -845,7 +845,7 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +878,7 @@
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <f>IF(A3=1,Skills!C2,IF(A3=2,Skills!C3,IF(A3=3,Skills!C4,IF(A3=4,Skills!C5,IF(A3=5,Skills!C6,IF(A3=6,Skills!C7,IF(A3=7,Skills!C8,IF(A3=8,Skills!C9,IF(A3=9,Skills!C10,"")))))))))</f>
@@ -894,7 +894,7 @@
       </c>
       <c r="F3" s="2">
         <f>IF(A3=1,Skills!F2,IF(A3=2,Skills!F3,IF(A3=3,Skills!F4,IF(A3=4,Skills!F5,IF(A3=5,Skills!F6,IF(A3=6,Skills!F7,IF(A3=7,Skills!F8,IF(A3=8,Skills!F9,IF(A3=9,Skills!F10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,24 +904,24 @@
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <f>IF(A5=1,Personality!C2,IF(A5=2,Personality!C3,IF(A5=3,Personality!C4,IF(A5=4,Personality!C5,IF(A5=5,Personality!C6,IF(A5=6,Personality!C7,IF(A5=7,Personality!C8,IF(A5=8,Personality!C9,IF(A5=9,Personality!C10,IF(A5=10,Personality!C11,IF(A5=11,Personality!C12,IF(A5=12,Personality!C13,IF(A5=13,Personality!C14,IF(A5=14,Personality!C15,IF(A5=15,Personality!C16,IF(A5=16,Personality!C17,IF(A5=17,Personality!C18,IF(A5=18,Personality!C19,IF(A5=19,Personality!C20,IF(A5=20,Personality!C21,IF(A5=21,Personality!C22,IF(A5=22,Personality!C23,IF(A5=23,Personality!C24,IF(A5=24,Personality!C25,""))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D5" s="2">
         <f>IF(A5=1,Personality!D2,IF(A5=2,Personality!D3,IF(A5=3,Personality!D4,IF(A5=4,Personality!D5,IF(A5=5,Personality!D6,IF(A5=6,Personality!D7,IF(A5=7,Personality!D8,IF(A5=8,Personality!D9,IF(A5=9,Personality!D10,IF(A5=10,Personality!D11,IF(A5=11,Personality!D12,IF(A5=12,Personality!D13,IF(A5=13,Personality!D14,IF(A5=14,Personality!D15,IF(A5=15,Personality!D16,IF(A5=16,Personality!D17,IF(A5=17,Personality!D18,IF(A5=18,Personality!D19,IF(A5=19,Personality!D20,IF(A5=20,Personality!D21,IF(A5=21,Personality!D22,IF(A5=22,Personality!D23,IF(A5=23,Personality!D24,IF(A5=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E5" s="2">
         <f>IF(A5=1,Personality!E2,IF(A5=2,Personality!E3,IF(A5=3,Personality!E4,IF(A5=4,Personality!E5,IF(A5=5,Personality!E6,IF(A5=6,Personality!E7,IF(A5=7,Personality!E8,IF(A5=8,Personality!E9,IF(A5=9,Personality!E10,IF(A5=10,Personality!E11,IF(A5=11,Personality!E12,IF(A5=12,Personality!E13,IF(A5=13,Personality!E14,IF(A5=14,Personality!E15,IF(A5=15,Personality!E16,IF(A5=16,Personality!E17,IF(A5=17,Personality!E18,IF(A5=18,Personality!E19,IF(A5=19,Personality!E20,IF(A5=20,Personality!E21,IF(A5=21,Personality!E22,IF(A5=22,Personality!E23,IF(A5=23,Personality!E24,IF(A5=24,Personality!E25,""))))))))))))))))))))))))</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F5" s="2">
         <f>IF(A5=1,Personality!F2,IF(A5=2,Personality!F3,IF(A5=3,Personality!F4,IF(A5=4,Personality!F5,IF(A5=5,Personality!F6,IF(A5=6,Personality!F7,IF(A5=7,Personality!F8,IF(A5=8,Personality!F9,IF(A5=9,Personality!F10,IF(A5=10,Personality!F11,IF(A5=11,Personality!F12,IF(A5=12,Personality!F13,IF(A5=13,Personality!F14,IF(A5=14,Personality!F15,IF(A5=15,Personality!F16,IF(A5=16,Personality!F17,IF(A5=17,Personality!F18,IF(A5=18,Personality!F19,IF(A5=19,Personality!F20,IF(A5=20,Personality!F21,IF(A5=21,Personality!F22,IF(A5=22,Personality!F23,IF(A5=23,Personality!F24,IF(A5=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -962,19 +962,19 @@
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <f>C3+C5+C7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ref="D10:F10" si="0">D3+D5+D7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -997,7 +997,7 @@
       </c>
       <c r="C12" s="7">
         <f>IF(C10=0,1,C10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="8">
         <f>IF(D10=0,1,D10)</f>
@@ -1005,11 +1005,11 @@
       </c>
       <c r="E12" s="8">
         <f>IF(E10=0,1,E10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="9">
         <f>IF(F10=0,1,F10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1311,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Tora decision. GER country file WIP Added Werner von Blomberg as Field Marshal.
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="18180" windowHeight="8085"/>
+    <workbookView xWindow="4200" yWindow="0" windowWidth="18180" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Skill level" sheetId="3" r:id="rId1"/>
@@ -355,15 +355,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$A$3" fmlaRange="Skills!$A$2:$A$10" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$A$3" fmlaRange="Skills!$A$2:$A$10" noThreeD="1" sel="3"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$5" fmlaRange="Personality!$B$2:$B$25" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$5" fmlaRange="Personality!$B$2:$B$25" noThreeD="1" sel="8" val="3"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$7" fmlaRange="Personality!$H$2:$H$26" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$7" fmlaRange="Personality!$H$2:$H$26" noThreeD="1" sel="22" val="15"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,7 +391,65 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF44EA9B-8541-4285-A248-4B9724E0DF30}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>85725</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1590675</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>409575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Vervolgkeuzelijst 5" descr="old guard" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -432,72 +490,14 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>85725</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>1590675</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>409575</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Vervolgkeuzelijst 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30E2922F-3E7C-48E6-96EE-D087350DCA50}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>84992</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>52022</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>1589942</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>413972</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -507,7 +507,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABEC48B4-6B87-4D7E-BB56-DB702CD1A93D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -846,7 +846,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,23 +878,23 @@
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <f>IF(A3=1,Skills!C2,IF(A3=2,Skills!C3,IF(A3=3,Skills!C4,IF(A3=4,Skills!C5,IF(A3=5,Skills!C6,IF(A3=6,Skills!C7,IF(A3=7,Skills!C8,IF(A3=8,Skills!C9,IF(A3=9,Skills!C10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <f>IF(A3=1,Skills!D2,IF(A3=2,Skills!D3,IF(A3=3,Skills!D4,IF(A3=4,Skills!D5,IF(A3=5,Skills!D6,IF(A3=6,Skills!D7,IF(A3=7,Skills!D8,IF(A3=8,Skills!D9,IF(A3=9,Skills!D10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
         <f>IF(A3=1,Skills!E2,IF(A3=2,Skills!E3,IF(A3=3,Skills!E4,IF(A3=4,Skills!E5,IF(A3=5,Skills!E6,IF(A3=6,Skills!E7,IF(A3=7,Skills!E8,IF(A3=8,Skills!E9,IF(A3=9,Skills!E10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
         <f>IF(A3=1,Skills!F2,IF(A3=2,Skills!F3,IF(A3=3,Skills!F4,IF(A3=4,Skills!F5,IF(A3=5,Skills!F6,IF(A3=6,Skills!F7,IF(A3=7,Skills!F8,IF(A3=8,Skills!F9,IF(A3=9,Skills!F10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,24 +904,24 @@
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <f>IF(A5=1,Personality!C2,IF(A5=2,Personality!C3,IF(A5=3,Personality!C4,IF(A5=4,Personality!C5,IF(A5=5,Personality!C6,IF(A5=6,Personality!C7,IF(A5=7,Personality!C8,IF(A5=8,Personality!C9,IF(A5=9,Personality!C10,IF(A5=10,Personality!C11,IF(A5=11,Personality!C12,IF(A5=12,Personality!C13,IF(A5=13,Personality!C14,IF(A5=14,Personality!C15,IF(A5=15,Personality!C16,IF(A5=16,Personality!C17,IF(A5=17,Personality!C18,IF(A5=18,Personality!C19,IF(A5=19,Personality!C20,IF(A5=20,Personality!C21,IF(A5=21,Personality!C22,IF(A5=22,Personality!C23,IF(A5=23,Personality!C24,IF(A5=24,Personality!C25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <f>IF(A5=1,Personality!D2,IF(A5=2,Personality!D3,IF(A5=3,Personality!D4,IF(A5=4,Personality!D5,IF(A5=5,Personality!D6,IF(A5=6,Personality!D7,IF(A5=7,Personality!D8,IF(A5=8,Personality!D9,IF(A5=9,Personality!D10,IF(A5=10,Personality!D11,IF(A5=11,Personality!D12,IF(A5=12,Personality!D13,IF(A5=13,Personality!D14,IF(A5=14,Personality!D15,IF(A5=15,Personality!D16,IF(A5=16,Personality!D17,IF(A5=17,Personality!D18,IF(A5=18,Personality!D19,IF(A5=19,Personality!D20,IF(A5=20,Personality!D21,IF(A5=21,Personality!D22,IF(A5=22,Personality!D23,IF(A5=23,Personality!D24,IF(A5=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <f>IF(A5=1,Personality!E2,IF(A5=2,Personality!E3,IF(A5=3,Personality!E4,IF(A5=4,Personality!E5,IF(A5=5,Personality!E6,IF(A5=6,Personality!E7,IF(A5=7,Personality!E8,IF(A5=8,Personality!E9,IF(A5=9,Personality!E10,IF(A5=10,Personality!E11,IF(A5=11,Personality!E12,IF(A5=12,Personality!E13,IF(A5=13,Personality!E14,IF(A5=14,Personality!E15,IF(A5=15,Personality!E16,IF(A5=16,Personality!E17,IF(A5=17,Personality!E18,IF(A5=18,Personality!E19,IF(A5=19,Personality!E20,IF(A5=20,Personality!E21,IF(A5=21,Personality!E22,IF(A5=22,Personality!E23,IF(A5=23,Personality!E24,IF(A5=24,Personality!E25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
         <f>IF(A5=1,Personality!F2,IF(A5=2,Personality!F3,IF(A5=3,Personality!F4,IF(A5=4,Personality!F5,IF(A5=5,Personality!F6,IF(A5=6,Personality!F7,IF(A5=7,Personality!F8,IF(A5=8,Personality!F9,IF(A5=9,Personality!F10,IF(A5=10,Personality!F11,IF(A5=11,Personality!F12,IF(A5=12,Personality!F13,IF(A5=13,Personality!F14,IF(A5=14,Personality!F15,IF(A5=15,Personality!F16,IF(A5=16,Personality!F17,IF(A5=17,Personality!F18,IF(A5=18,Personality!F19,IF(A5=19,Personality!F20,IF(A5=20,Personality!F21,IF(A5=21,Personality!F22,IF(A5=22,Personality!F23,IF(A5=23,Personality!F24,IF(A5=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
     </row>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
         <f>IF(A7=1,Personality!I2,IF(A7=2,Personality!I3,IF(A7=3,Personality!I4,IF(A7=4,Personality!I5,IF(A7=5,Personality!I6,IF(A7=6,Personality!I7,IF(A7=7,Personality!I8,IF(A7=8,Personality!I9,IF(A7=9,Personality!I10,IF(A7=10,Personality!I11,IF(A7=11,Personality!I12,IF(A7=12,Personality!I13,IF(A7=13,Personality!I14,IF(A7=14,Personality!I15,IF(A7=15,Personality!I16,IF(A7=16,Personality!I17,IF(A7=17,Personality!I18,IF(A7=18,Personality!I19,IF(A7=19,Personality!I20,IF(A7=20,Personality!I21,IF(A7=21,Personality!I22,IF(A7=22,Personality!I23,IF(A7=23,Personality!I24,IF(A7=24,Personality!I25,IF(A7=25,Personality!I26,"")))))))))))))))))))))))))</f>
@@ -939,11 +939,11 @@
       </c>
       <c r="D7" s="2">
         <f>IF(A7=1,Personality!J2,IF(A7=2,Personality!J3,IF(A7=3,Personality!J4,IF(A7=4,Personality!J5,IF(A7=5,Personality!J6,IF(A7=6,Personality!J7,IF(A7=7,Personality!J8,IF(A7=8,Personality!J9,IF(A7=9,Personality!J10,IF(A7=10,Personality!J11,IF(A7=11,Personality!J12,IF(A7=12,Personality!J13,IF(A7=13,Personality!J14,IF(A7=14,Personality!J15,IF(A7=15,Personality!J16,IF(A7=16,Personality!J17,IF(A7=17,Personality!J18,IF(A7=18,Personality!J19,IF(A7=19,Personality!J20,IF(A7=20,Personality!J21,IF(A7=21,Personality!J22,IF(A7=22,Personality!J23,IF(A7=23,Personality!J24,IF(A7=24,Personality!J25,IF(A7=25,Personality!J26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <f>IF(A7=1,Personality!K2,IF(A7=2,Personality!K3,IF(A7=3,Personality!K4,IF(A7=4,Personality!K5,IF(A7=5,Personality!K6,IF(A7=6,Personality!K7,IF(A7=7,Personality!K8,IF(A7=8,Personality!K9,IF(A7=9,Personality!K10,IF(A7=10,Personality!K11,IF(A7=11,Personality!K12,IF(A7=12,Personality!K13,IF(A7=13,Personality!K14,IF(A7=14,Personality!K15,IF(A7=15,Personality!K16,IF(A7=16,Personality!K17,IF(A7=17,Personality!K18,IF(A7=18,Personality!K19,IF(A7=19,Personality!K20,IF(A7=20,Personality!K21,IF(A7=21,Personality!K22,IF(A7=22,Personality!K23,IF(A7=23,Personality!K24,IF(A7=24,Personality!K25,IF(A7=25,Personality!K26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
         <f>IF(A7=1,Personality!L2,IF(A7=2,Personality!L3,IF(A7=3,Personality!L4,IF(A7=4,Personality!L5,IF(A7=5,Personality!L6,IF(A7=6,Personality!L7,IF(A7=7,Personality!L8,IF(A7=8,Personality!L9,IF(A7=9,Personality!L10,IF(A7=10,Personality!L11,IF(A7=11,Personality!L12,IF(A7=12,Personality!L13,IF(A7=13,Personality!L14,IF(A7=14,Personality!L15,IF(A7=15,Personality!L16,IF(A7=16,Personality!L17,IF(A7=17,Personality!L18,IF(A7=18,Personality!L19,IF(A7=19,Personality!L20,IF(A7=20,Personality!L21,IF(A7=21,Personality!L22,IF(A7=22,Personality!L23,IF(A7=23,Personality!L24,IF(A7=24,Personality!L25,IF(A7=25,Personality!L26,"")))))))))))))))))))))))))</f>
@@ -962,19 +962,19 @@
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <f>C3+C5+C7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ref="D10:F10" si="0">D3+D5+D7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -997,19 +997,19 @@
       </c>
       <c r="C12" s="7">
         <f>IF(C10=0,1,C10)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="8">
         <f>IF(D10=0,1,D10)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="8">
         <f>IF(E10=0,1,E10)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12" s="9">
         <f>IF(F10=0,1,F10)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,16 +1198,16 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,13 +1648,13 @@
         <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>12</v>
@@ -1683,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
@@ -1698,13 +1698,13 @@
         <v>2</v>
       </c>
       <c r="J11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="3">
         <v>2</v>
       </c>
       <c r="L11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1715,13 +1715,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -1733,13 +1733,13 @@
         <v>2</v>
       </c>
       <c r="J12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="3">
         <v>3</v>
       </c>
       <c r="L12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>15</v>
       </c>
       <c r="I13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="3">
         <v>0</v>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>16</v>
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
@@ -1911,7 +1911,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -1995,7 +1995,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
@@ -2033,19 +2033,19 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="3">
         <v>0</v>
@@ -2068,10 +2068,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
@@ -2083,13 +2083,13 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
       </c>
       <c r="L22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2118,10 +2118,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Added 2 more personality choices to Skill levels
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\maver\Documents\Paradox Interactive\Hearts of Iron IV\mod\Blackice-WIP-v2.5\BICE modfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruud\Documents\Paradox Interactive\Hearts of Iron IV\mod\blackice-hoi4_v2.5 WIP\BICE modfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,9 +17,9 @@
     <sheet name="Personality" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$A$1:$G$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$B$2:$H$16</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Old G</t>
   </si>
@@ -137,12 +137,18 @@
   </si>
   <si>
     <t>Personality 2</t>
+  </si>
+  <si>
+    <t>Choose Personality 3</t>
+  </si>
+  <si>
+    <t>Calc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +225,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -336,6 +348,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -355,15 +374,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$A$3" fmlaRange="Skills!$A$2:$A$10" noThreeD="1" sel="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="3" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$5" fmlaRange="Personality!$B$2:$B$25" noThreeD="1" sel="8" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="16" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$7" fmlaRange="Personality!$H$2:$H$26" noThreeD="1" sel="22" val="15"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="8" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="16" fmlaLink="$B$10" fmlaRange="Personality!$H$2:$H$26" sel="1" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,15 +395,15 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>2</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>1571625</xdr:colOff>
-          <xdr:row>2</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>409575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -391,7 +414,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -430,26 +453,26 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>85725</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>1590675</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>409575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Vervolgkeuzelijst 5" descr="old guard" hidden="1">
+            <xdr:cNvPr id="1035" name="Vervolgkeuzelijst 11" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
+                  <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -488,26 +511,81 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>85725</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>0</xdr:col>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>1590675</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>409575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1035" name="Vervolgkeuzelijst 11" hidden="1">
+            <xdr:cNvPr id="1029" name="Vervolgkeuzelijst 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1035"/>
+                  <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1581150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>400050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Drop Down 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -843,174 +921,754 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad3"/>
-  <dimension ref="A2:G12"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+    </row>
+    <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <f>IF(A3=1,Skills!C2,IF(A3=2,Skills!C3,IF(A3=3,Skills!C4,IF(A3=4,Skills!C5,IF(A3=5,Skills!C6,IF(A3=6,Skills!C7,IF(A3=7,Skills!C8,IF(A3=8,Skills!C9,IF(A3=9,Skills!C10,"")))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <f>IF(A3=1,Skills!D2,IF(A3=2,Skills!D3,IF(A3=3,Skills!D4,IF(A3=4,Skills!D5,IF(A3=5,Skills!D6,IF(A3=6,Skills!D7,IF(A3=7,Skills!D8,IF(A3=8,Skills!D9,IF(A3=9,Skills!D10,"")))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="E3" s="2">
-        <f>IF(A3=1,Skills!E2,IF(A3=2,Skills!E3,IF(A3=3,Skills!E4,IF(A3=4,Skills!E5,IF(A3=5,Skills!E6,IF(A3=6,Skills!E7,IF(A3=7,Skills!E8,IF(A3=8,Skills!E9,IF(A3=9,Skills!E10,"")))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <f>IF(A3=1,Skills!F2,IF(A3=2,Skills!F3,IF(A3=3,Skills!F4,IF(A3=4,Skills!F5,IF(A3=5,Skills!F6,IF(A3=6,Skills!F7,IF(A3=7,Skills!F8,IF(A3=8,Skills!F9,IF(A3=9,Skills!F10,"")))))))))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="D4" s="2">
+        <f>IF(B4=1,Skills!C2,IF(B4=2,Skills!C3,IF(B4=3,Skills!C4,IF(B4=4,Skills!C5,IF(B4=5,Skills!C6,IF(B4=6,Skills!C7,IF(B4=7,Skills!C8,IF(B4=8,Skills!C9,IF(B4=9,Skills!C10,"")))))))))</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <f>IF(B4=1,Skills!D2,IF(B4=2,Skills!D3,IF(B4=3,Skills!D4,IF(B4=4,Skills!D5,IF(B4=5,Skills!D6,IF(B4=6,Skills!D7,IF(B4=7,Skills!D8,IF(B4=8,Skills!D9,IF(B4=9,Skills!D10,"")))))))))</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <f>IF(B4=1,Skills!E2,IF(B4=2,Skills!E3,IF(B4=3,Skills!E4,IF(B4=4,Skills!E5,IF(B4=5,Skills!E6,IF(B4=6,Skills!E7,IF(B4=7,Skills!E8,IF(B4=8,Skills!E9,IF(B4=9,Skills!E10,"")))))))))</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <f>IF(B4=1,Skills!F2,IF(B4=2,Skills!F3,IF(B4=3,Skills!F4,IF(B4=4,Skills!F5,IF(B4=5,Skills!F6,IF(B4=6,Skills!F7,IF(B4=7,Skills!F8,IF(B4=8,Skills!F9,IF(B4=9,Skills!F10,"")))))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+    </row>
+    <row r="6" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
-        <f>IF(A5=1,Personality!C2,IF(A5=2,Personality!C3,IF(A5=3,Personality!C4,IF(A5=4,Personality!C5,IF(A5=5,Personality!C6,IF(A5=6,Personality!C7,IF(A5=7,Personality!C8,IF(A5=8,Personality!C9,IF(A5=9,Personality!C10,IF(A5=10,Personality!C11,IF(A5=11,Personality!C12,IF(A5=12,Personality!C13,IF(A5=13,Personality!C14,IF(A5=14,Personality!C15,IF(A5=15,Personality!C16,IF(A5=16,Personality!C17,IF(A5=17,Personality!C18,IF(A5=18,Personality!C19,IF(A5=19,Personality!C20,IF(A5=20,Personality!C21,IF(A5=21,Personality!C22,IF(A5=22,Personality!C23,IF(A5=23,Personality!C24,IF(A5=24,Personality!C25,""))))))))))))))))))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <f>IF(A5=1,Personality!D2,IF(A5=2,Personality!D3,IF(A5=3,Personality!D4,IF(A5=4,Personality!D5,IF(A5=5,Personality!D6,IF(A5=6,Personality!D7,IF(A5=7,Personality!D8,IF(A5=8,Personality!D9,IF(A5=9,Personality!D10,IF(A5=10,Personality!D11,IF(A5=11,Personality!D12,IF(A5=12,Personality!D13,IF(A5=13,Personality!D14,IF(A5=14,Personality!D15,IF(A5=15,Personality!D16,IF(A5=16,Personality!D17,IF(A5=17,Personality!D18,IF(A5=18,Personality!D19,IF(A5=19,Personality!D20,IF(A5=20,Personality!D21,IF(A5=21,Personality!D22,IF(A5=22,Personality!D23,IF(A5=23,Personality!D24,IF(A5=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <f>IF(A5=1,Personality!E2,IF(A5=2,Personality!E3,IF(A5=3,Personality!E4,IF(A5=4,Personality!E5,IF(A5=5,Personality!E6,IF(A5=6,Personality!E7,IF(A5=7,Personality!E8,IF(A5=8,Personality!E9,IF(A5=9,Personality!E10,IF(A5=10,Personality!E11,IF(A5=11,Personality!E12,IF(A5=12,Personality!E13,IF(A5=13,Personality!E14,IF(A5=14,Personality!E15,IF(A5=15,Personality!E16,IF(A5=16,Personality!E17,IF(A5=17,Personality!E18,IF(A5=18,Personality!E19,IF(A5=19,Personality!E20,IF(A5=20,Personality!E21,IF(A5=21,Personality!E22,IF(A5=22,Personality!E23,IF(A5=23,Personality!E24,IF(A5=24,Personality!E25,""))))))))))))))))))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <f>IF(A5=1,Personality!F2,IF(A5=2,Personality!F3,IF(A5=3,Personality!F4,IF(A5=4,Personality!F5,IF(A5=5,Personality!F6,IF(A5=6,Personality!F7,IF(A5=7,Personality!F8,IF(A5=8,Personality!F9,IF(A5=9,Personality!F10,IF(A5=10,Personality!F11,IF(A5=11,Personality!F12,IF(A5=12,Personality!F13,IF(A5=13,Personality!F14,IF(A5=14,Personality!F15,IF(A5=15,Personality!F16,IF(A5=16,Personality!F17,IF(A5=17,Personality!F18,IF(A5=18,Personality!F19,IF(A5=19,Personality!F20,IF(A5=20,Personality!F21,IF(A5=21,Personality!F22,IF(A5=22,Personality!F23,IF(A5=23,Personality!F24,IF(A5=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <f>IF(B6=1,Personality!C2,IF(B6=2,Personality!C3,IF(B6=3,Personality!C4,IF(B6=4,Personality!C5,IF(B6=5,Personality!C6,IF(B6=6,Personality!C7,IF(B6=7,Personality!C8,IF(B6=8,Personality!C9,IF(B6=9,Personality!C10,IF(B6=10,Personality!C11,IF(B6=11,Personality!C12,IF(B6=12,Personality!C13,IF(B6=13,Personality!C14,IF(B6=14,Personality!C15,IF(B6=15,Personality!C16,IF(B6=16,Personality!C17,IF(B6=17,Personality!C18,IF(B6=18,Personality!C19,IF(B6=19,Personality!C20,IF(B6=20,Personality!C21,IF(B6=21,Personality!C22,IF(B6=22,Personality!C23,IF(B6=23,Personality!C24,IF(B6=24,Personality!C25,""))))))))))))))))))))))))</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <f>IF(B6=1,Personality!D2,IF(B6=2,Personality!D3,IF(B6=3,Personality!D4,IF(B6=4,Personality!D5,IF(B6=5,Personality!D6,IF(B6=6,Personality!D7,IF(B6=7,Personality!D8,IF(B6=8,Personality!D9,IF(B6=9,Personality!D10,IF(B6=10,Personality!D11,IF(B6=11,Personality!D12,IF(B6=12,Personality!D13,IF(B6=13,Personality!D14,IF(B6=14,Personality!D15,IF(B6=15,Personality!D16,IF(B6=16,Personality!D17,IF(B6=17,Personality!D18,IF(B6=18,Personality!D19,IF(B6=19,Personality!D20,IF(B6=20,Personality!D21,IF(B6=21,Personality!D22,IF(B6=22,Personality!D23,IF(B6=23,Personality!D24,IF(B6=24,Personality!D25,""))))))))))))))))))))))))</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <f>IF(B6=1,Personality!E2,IF(B6=2,Personality!E3,IF(B6=3,Personality!E4,IF(B6=4,Personality!E5,IF(B6=5,Personality!E6,IF(B6=6,Personality!E7,IF(B6=7,Personality!E8,IF(B6=8,Personality!E9,IF(B6=9,Personality!E10,IF(B6=10,Personality!E11,IF(B6=11,Personality!E12,IF(B6=12,Personality!E13,IF(B6=13,Personality!E14,IF(B6=14,Personality!E15,IF(B6=15,Personality!E16,IF(B6=16,Personality!E17,IF(B6=17,Personality!E18,IF(B6=18,Personality!E19,IF(B6=19,Personality!E20,IF(B6=20,Personality!E21,IF(B6=21,Personality!E22,IF(B6=22,Personality!E23,IF(B6=23,Personality!E24,IF(B6=24,Personality!E25,""))))))))))))))))))))))))</f>
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <f>IF(B6=1,Personality!F2,IF(B6=2,Personality!F3,IF(B6=3,Personality!F4,IF(B6=4,Personality!F5,IF(B6=5,Personality!F6,IF(B6=6,Personality!F7,IF(B6=7,Personality!F8,IF(B6=8,Personality!F9,IF(B6=9,Personality!F10,IF(B6=10,Personality!F11,IF(B6=11,Personality!F12,IF(B6=12,Personality!F13,IF(B6=13,Personality!F14,IF(B6=14,Personality!F15,IF(B6=15,Personality!F16,IF(B6=16,Personality!F17,IF(B6=17,Personality!F18,IF(B6=18,Personality!F19,IF(B6=19,Personality!F20,IF(B6=20,Personality!F21,IF(B6=21,Personality!F22,IF(B6=22,Personality!F23,IF(B6=23,Personality!F24,IF(B6=24,Personality!F25,""))))))))))))))))))))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2">
-        <f>IF(A7=1,Personality!I2,IF(A7=2,Personality!I3,IF(A7=3,Personality!I4,IF(A7=4,Personality!I5,IF(A7=5,Personality!I6,IF(A7=6,Personality!I7,IF(A7=7,Personality!I8,IF(A7=8,Personality!I9,IF(A7=9,Personality!I10,IF(A7=10,Personality!I11,IF(A7=11,Personality!I12,IF(A7=12,Personality!I13,IF(A7=13,Personality!I14,IF(A7=14,Personality!I15,IF(A7=15,Personality!I16,IF(A7=16,Personality!I17,IF(A7=17,Personality!I18,IF(A7=18,Personality!I19,IF(A7=19,Personality!I20,IF(A7=20,Personality!I21,IF(A7=21,Personality!I22,IF(A7=22,Personality!I23,IF(A7=23,Personality!I24,IF(A7=24,Personality!I25,IF(A7=25,Personality!I26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <f>IF(A7=1,Personality!J2,IF(A7=2,Personality!J3,IF(A7=3,Personality!J4,IF(A7=4,Personality!J5,IF(A7=5,Personality!J6,IF(A7=6,Personality!J7,IF(A7=7,Personality!J8,IF(A7=8,Personality!J9,IF(A7=9,Personality!J10,IF(A7=10,Personality!J11,IF(A7=11,Personality!J12,IF(A7=12,Personality!J13,IF(A7=13,Personality!J14,IF(A7=14,Personality!J15,IF(A7=15,Personality!J16,IF(A7=16,Personality!J17,IF(A7=17,Personality!J18,IF(A7=18,Personality!J19,IF(A7=19,Personality!J20,IF(A7=20,Personality!J21,IF(A7=21,Personality!J22,IF(A7=22,Personality!J23,IF(A7=23,Personality!J24,IF(A7=24,Personality!J25,IF(A7=25,Personality!J26,"")))))))))))))))))))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <f>IF(A7=1,Personality!K2,IF(A7=2,Personality!K3,IF(A7=3,Personality!K4,IF(A7=4,Personality!K5,IF(A7=5,Personality!K6,IF(A7=6,Personality!K7,IF(A7=7,Personality!K8,IF(A7=8,Personality!K9,IF(A7=9,Personality!K10,IF(A7=10,Personality!K11,IF(A7=11,Personality!K12,IF(A7=12,Personality!K13,IF(A7=13,Personality!K14,IF(A7=14,Personality!K15,IF(A7=15,Personality!K16,IF(A7=16,Personality!K17,IF(A7=17,Personality!K18,IF(A7=18,Personality!K19,IF(A7=19,Personality!K20,IF(A7=20,Personality!K21,IF(A7=21,Personality!K22,IF(A7=22,Personality!K23,IF(A7=23,Personality!K24,IF(A7=24,Personality!K25,IF(A7=25,Personality!K26,"")))))))))))))))))))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <f>IF(A7=1,Personality!L2,IF(A7=2,Personality!L3,IF(A7=3,Personality!L4,IF(A7=4,Personality!L5,IF(A7=5,Personality!L6,IF(A7=6,Personality!L7,IF(A7=7,Personality!L8,IF(A7=8,Personality!L9,IF(A7=9,Personality!L10,IF(A7=10,Personality!L11,IF(A7=11,Personality!L12,IF(A7=12,Personality!L13,IF(A7=13,Personality!L14,IF(A7=14,Personality!L15,IF(A7=15,Personality!L16,IF(A7=16,Personality!L17,IF(A7=17,Personality!L18,IF(A7=18,Personality!L19,IF(A7=19,Personality!L20,IF(A7=20,Personality!L21,IF(A7=21,Personality!L22,IF(A7=22,Personality!L23,IF(A7=23,Personality!L24,IF(A7=24,Personality!L25,IF(A7=25,Personality!L26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="3">
-        <f>C3+C5+C7</f>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+    </row>
+    <row r="8" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="5">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <f>IF(B8=1,Personality!I2,IF(B8=2,Personality!I3,IF(B8=3,Personality!I4,IF(B8=4,Personality!I5,IF(B8=5,Personality!I6,IF(B8=6,Personality!I7,IF(B8=7,Personality!I8,IF(B8=8,Personality!I9,IF(B8=9,Personality!I10,IF(B8=10,Personality!I11,IF(B8=11,Personality!I12,IF(B8=12,Personality!I13,IF(B8=13,Personality!I14,IF(B8=14,Personality!I15,IF(B8=15,Personality!I16,IF(B8=16,Personality!I17,IF(B8=17,Personality!I18,IF(B8=18,Personality!I19,IF(B8=19,Personality!I20,IF(B8=20,Personality!I21,IF(B8=21,Personality!I22,IF(B8=22,Personality!I23,IF(B8=23,Personality!I24,IF(B8=24,Personality!I25,IF(B8=25,Personality!I26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <f>IF(B8=1,Personality!J2,IF(B8=2,Personality!J3,IF(B8=3,Personality!J4,IF(B8=4,Personality!J5,IF(B8=5,Personality!J6,IF(B8=6,Personality!J7,IF(B8=7,Personality!J8,IF(B8=8,Personality!J9,IF(B8=9,Personality!J10,IF(B8=10,Personality!J11,IF(B8=11,Personality!J12,IF(B8=12,Personality!J13,IF(B8=13,Personality!J14,IF(B8=14,Personality!J15,IF(B8=15,Personality!J16,IF(B8=16,Personality!J17,IF(B8=17,Personality!J18,IF(B8=18,Personality!J19,IF(B8=19,Personality!J20,IF(B8=20,Personality!J21,IF(B8=21,Personality!J22,IF(B8=22,Personality!J23,IF(B8=23,Personality!J24,IF(B8=24,Personality!J25,IF(B8=25,Personality!J26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <f>IF(B8=1,Personality!K2,IF(B8=2,Personality!K3,IF(B8=3,Personality!K4,IF(B8=4,Personality!K5,IF(B8=5,Personality!K6,IF(B8=6,Personality!K7,IF(B8=7,Personality!K8,IF(B8=8,Personality!K9,IF(B8=9,Personality!K10,IF(B8=10,Personality!K11,IF(B8=11,Personality!K12,IF(B8=12,Personality!K13,IF(B8=13,Personality!K14,IF(B8=14,Personality!K15,IF(B8=15,Personality!K16,IF(B8=16,Personality!K17,IF(B8=17,Personality!K18,IF(B8=18,Personality!K19,IF(B8=19,Personality!K20,IF(B8=20,Personality!K21,IF(B8=21,Personality!K22,IF(B8=22,Personality!K23,IF(B8=23,Personality!K24,IF(B8=24,Personality!K25,IF(B8=25,Personality!K26,"")))))))))))))))))))))))))</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f>IF(B8=1,Personality!L2,IF(B8=2,Personality!L3,IF(B8=3,Personality!L4,IF(B8=4,Personality!L5,IF(B8=5,Personality!L6,IF(B8=6,Personality!L7,IF(B8=7,Personality!L8,IF(B8=8,Personality!L9,IF(B8=9,Personality!L10,IF(B8=10,Personality!L11,IF(B8=11,Personality!L12,IF(B8=12,Personality!L13,IF(B8=13,Personality!L14,IF(B8=14,Personality!L15,IF(B8=15,Personality!L16,IF(B8=16,Personality!L17,IF(B8=17,Personality!L18,IF(B8=18,Personality!L19,IF(B8=19,Personality!L20,IF(B8=20,Personality!L21,IF(B8=21,Personality!L22,IF(B8=22,Personality!L23,IF(B8=23,Personality!L24,IF(B8=24,Personality!L25,IF(B8=25,Personality!L26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+    </row>
+    <row r="10" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <f>IF(B10=1,Personality!I2,IF(B10=2,Personality!I3,IF(B10=3,Personality!I4,IF(B10=4,Personality!I5,IF(B10=5,Personality!I6,IF(B10=6,Personality!I7,IF(B10=7,Personality!I8,IF(B10=8,Personality!I8,IF(B10=9,Personality!I10,IF(B10=10,Personality!I11,IF(B10=11,Personality!I12,IF(B10=12,Personality!I13,IF(B10=13,Personality!I14,IF(B10=14,Personality!I15,IF(B10=15,Personality!I16,IF(B10=16,Personality!I17,IF(B10=17,Personality!I18,IF(B10=18,Personality!I19,IF(B10=19,Personality!I20,IF(B10=20,Personality!I21,IF(B10=21,Personality!I22,IF(B10=22,Personality!I23,IF(B10=23,Personality!I24,IF(B10=24,Personality!I25,IF(B10=25,Personality!I26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f>IF(B10=1,Personality!J2,IF(B10=2,Personality!J3,IF(B10=3,Personality!J4,IF(B10=4,Personality!J5,IF(B10=5,Personality!J6,IF(B10=6,Personality!J7,IF(B10=7,Personality!J8,IF(B10=8,Personality!J8,IF(B10=9,Personality!J10,IF(B10=10,Personality!J11,IF(B10=11,Personality!J12,IF(B10=12,Personality!J13,IF(B10=13,Personality!J14,IF(B10=14,Personality!J15,IF(B10=15,Personality!J16,IF(B10=16,Personality!J17,IF(B10=17,Personality!J18,IF(B10=18,Personality!J19,IF(B10=19,Personality!J20,IF(B10=20,Personality!J21,IF(B10=21,Personality!J22,IF(B10=22,Personality!J23,IF(B10=23,Personality!J24,IF(B10=24,Personality!J25,IF(B10=25,Personality!J26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>IF(B10=1,Personality!K2,IF(B10=2,Personality!K3,IF(B10=3,Personality!K4,IF(B10=4,Personality!K5,IF(B10=5,Personality!K6,IF(B10=6,Personality!K7,IF(B10=7,Personality!K8,IF(B10=8,Personality!K8,IF(B10=9,Personality!K10,IF(B10=10,Personality!K11,IF(B10=11,Personality!K12,IF(B10=12,Personality!K13,IF(B10=13,Personality!K14,IF(B10=14,Personality!K15,IF(B10=15,Personality!K16,IF(B10=16,Personality!K17,IF(B10=17,Personality!K18,IF(B10=18,Personality!K19,IF(B10=19,Personality!K20,IF(B10=20,Personality!K21,IF(B10=21,Personality!K22,IF(B10=22,Personality!K23,IF(B10=23,Personality!K24,IF(B10=24,Personality!K25,IF(B10=25,Personality!K26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f>IF(B10=1,Personality!K2,IF(B10=2,Personality!K3,IF(B10=3,Personality!K4,IF(B10=4,Personality!K5,IF(B10=5,Personality!K6,IF(B10=6,Personality!K7,IF(B10=7,Personality!K8,IF(B10=8,Personality!K8,IF(B10=9,Personality!K10,IF(B10=10,Personality!K11,IF(B10=11,Personality!K12,IF(B10=12,Personality!K13,IF(B10=13,Personality!K14,IF(B10=14,Personality!K15,IF(B10=15,Personality!K16,IF(B10=16,Personality!K17,IF(B10=17,Personality!K18,IF(B10=18,Personality!K19,IF(B10=19,Personality!K20,IF(B10=20,Personality!K21,IF(B10=21,Personality!K22,IF(B10=22,Personality!K23,IF(B10=23,Personality!K24,IF(B10=24,Personality!K25,IF(B10=25,Personality!K26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="14"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="14"/>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3">
+        <f>D4+D6+D8+D10</f>
         <v>3</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:F10" si="0">D3+D5+D7</f>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13:G13" si="0">E4+E6+E8+E10</f>
         <v>3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="C11" s="10" t="s">
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+    </row>
+    <row r="14" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+    </row>
+    <row r="15" spans="1:25" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="17"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="7">
-        <f>IF(C10=0,1,C10)</f>
+      <c r="D15" s="7">
+        <f>IF(D13=0,1,D13)</f>
         <v>3</v>
       </c>
-      <c r="D12" s="8">
-        <f>IF(D10=0,1,D10)</f>
+      <c r="E15" s="8">
+        <f>IF(E13=0,1,E13)</f>
         <v>3</v>
       </c>
-      <c r="E12" s="8">
-        <f>IF(E10=0,1,E10)</f>
+      <c r="F15" s="8">
+        <f>IF(F13=0,1,F13)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="9">
-        <f>IF(F10=0,1,F10)</f>
+      <c r="G15" s="9">
+        <f>IF(G13=0,1,G13)</f>
         <v>3</v>
       </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="14"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1022,19 +1680,19 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId4" name="Drop Down 4">
+            <control shapeId="1028" r:id="rId4" name="Vervolgkeuzelijst 4">
               <controlPr defaultSize="0" print="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>0</xdr:col>
+                    <xdr:col>1</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:row>3</xdr:row>
                     <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>0</xdr:col>
+                    <xdr:col>1</xdr:col>
                     <xdr:colOff>1571625</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:row>3</xdr:row>
                     <xdr:rowOff>409575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1044,19 +1702,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId5" name="Drop Down 5">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0" altText="old guard">
+            <control shapeId="1035" r:id="rId5" name="Vervolgkeuzelijst 11">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>0</xdr:col>
+                    <xdr:col>1</xdr:col>
                     <xdr:colOff>85725</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>0</xdr:col>
+                    <xdr:col>1</xdr:col>
                     <xdr:colOff>1590675</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>409575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1066,20 +1724,42 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId6" name="Drop Down 11">
+            <control shapeId="1029" r:id="rId6" name="Vervolgkeuzelijst 5">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" altText="">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1590675</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>409575</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId7" name="Drop Down 12">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>1590675</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>409575</xdr:rowOff>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1581150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>400050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1098,7 +1778,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,16 +1896,16 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1312,13 +1992,13 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1361,7 +2041,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3">
@@ -1376,7 +2056,7 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I2" s="3">
@@ -1396,7 +2076,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3">
@@ -1411,7 +2091,7 @@
       <c r="F3" s="3">
         <v>-1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="3">
@@ -1431,7 +2111,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3">
@@ -1446,7 +2126,7 @@
       <c r="F4" s="3">
         <v>-1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="3">
@@ -1466,7 +2146,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3">
@@ -1481,7 +2161,7 @@
       <c r="F5" s="3">
         <v>-1</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="3">
@@ -1501,7 +2181,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3">
@@ -1516,7 +2196,7 @@
       <c r="F6" s="3">
         <v>-1</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="15" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="3">
@@ -1536,7 +2216,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3">
@@ -1551,7 +2231,7 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="15" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="3">
@@ -1571,7 +2251,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3">
@@ -1586,7 +2266,7 @@
       <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="3">
@@ -1606,14 +2286,14 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
@@ -1621,7 +2301,7 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="3">
@@ -1641,22 +2321,22 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="3">
@@ -1676,22 +2356,22 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>2</v>
       </c>
       <c r="D11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="3">
@@ -1711,7 +2391,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3">
@@ -1721,12 +2401,12 @@
         <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="3">
@@ -1746,7 +2426,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3">
@@ -1756,12 +2436,12 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="3">
@@ -1781,7 +2461,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3">
@@ -1796,7 +2476,7 @@
       <c r="F14" s="3">
         <v>-1</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="3">
@@ -1816,7 +2496,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3">
@@ -1826,12 +2506,12 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="3">
@@ -1851,7 +2531,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3">
@@ -1866,7 +2546,7 @@
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="15" t="s">
         <v>18</v>
       </c>
       <c r="I16" s="3">
@@ -1876,32 +2556,32 @@
         <v>0</v>
       </c>
       <c r="K16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="3">
@@ -1921,14 +2601,14 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -1936,17 +2616,17 @@
       <c r="F18" s="3">
         <v>0</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L18" s="3">
         <v>0</v>
@@ -1956,7 +2636,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3">
@@ -1966,19 +2646,19 @@
         <v>0</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="15" t="s">
         <v>21</v>
       </c>
       <c r="I19" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J19" s="3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K19" s="3">
         <v>0</v>
@@ -1991,7 +2671,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="3">
@@ -2006,7 +2686,7 @@
       <c r="F20" s="3">
         <v>0</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="3">
@@ -2016,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L20" s="3">
         <v>0</v>
@@ -2026,7 +2706,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="3">
@@ -2041,7 +2721,7 @@
       <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="15" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="3">
@@ -2061,7 +2741,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3">
@@ -2076,7 +2756,7 @@
       <c r="F22" s="3">
         <v>0</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="3">
@@ -2096,7 +2776,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="3">
@@ -2111,7 +2791,7 @@
       <c r="F23" s="3">
         <v>0</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="15" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="3">
@@ -2131,22 +2811,22 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="15" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="3">
@@ -2166,7 +2846,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="3">
@@ -2181,25 +2861,25 @@
       <c r="F25" s="3">
         <v>0</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="15" t="s">
         <v>27</v>
       </c>
       <c r="I25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="3">
         <v>1</v>
       </c>
       <c r="K25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="15" t="s">
         <v>28</v>
       </c>
       <c r="I26" s="3">

</xml_diff>

<commit_message>
Added WTT_CHINA due to US-generals USA countryfile finished Corrected US-genreals in events/nf Deleted USA_tag Deleted SAP_conservatism flags
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruud\Documents\Paradox Interactive\Hearts of Iron IV\mod\blackice-hoi4_v2.5 WIP\BICE modfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\maver\Documents\Paradox Interactive\Hearts of Iron IV\mod\Blackice-WIP-v2.5\BICE modfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="0" windowWidth="18180" windowHeight="8085"/>
+    <workbookView xWindow="6300" yWindow="0" windowWidth="18180" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Skill level" sheetId="3" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="Personality" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$B$2:$H$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$B$2:$H$18</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Old G</t>
   </si>
@@ -143,12 +143,15 @@
   </si>
   <si>
     <t>Calc.</t>
+  </si>
+  <si>
+    <t>Choose Personality 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,19 +377,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="16" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="22" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="8" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="7" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="16" fmlaLink="$B$10" fmlaRange="Personality!$H$2:$H$26" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="16" fmlaLink="$B$12" fmlaRange="Personality!$H$2:$H$26" sel="1" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,7 +421,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -472,7 +479,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -530,7 +537,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -587,6 +594,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -617,6 +627,59 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1504950" cy="361950"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="Drop Down 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAEA6A3-B0FE-4734-AE4B-730501C5812B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -921,10 +984,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad3"/>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,23 +1085,23 @@
     <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <f>IF(B4=1,Skills!C2,IF(B4=2,Skills!C3,IF(B4=3,Skills!C4,IF(B4=4,Skills!C5,IF(B4=5,Skills!C6,IF(B4=6,Skills!C7,IF(B4=7,Skills!C8,IF(B4=8,Skills!C9,IF(B4=9,Skills!C10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <f>IF(B4=1,Skills!D2,IF(B4=2,Skills!D3,IF(B4=3,Skills!D4,IF(B4=4,Skills!D5,IF(B4=5,Skills!D6,IF(B4=6,Skills!D7,IF(B4=7,Skills!D8,IF(B4=8,Skills!D9,IF(B4=9,Skills!D10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
         <f>IF(B4=1,Skills!E2,IF(B4=2,Skills!E3,IF(B4=3,Skills!E4,IF(B4=4,Skills!E5,IF(B4=5,Skills!E6,IF(B4=6,Skills!E7,IF(B4=7,Skills!E8,IF(B4=8,Skills!E9,IF(B4=9,Skills!E10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
         <f>IF(B4=1,Skills!F2,IF(B4=2,Skills!F3,IF(B4=3,Skills!F4,IF(B4=4,Skills!F5,IF(B4=5,Skills!F6,IF(B4=6,Skills!F7,IF(B4=7,Skills!F8,IF(B4=8,Skills!F9,IF(B4=9,Skills!F10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -1084,7 +1147,7 @@
     <row r="6" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -1093,7 +1156,7 @@
       </c>
       <c r="E6" s="2">
         <f>IF(B6=1,Personality!D2,IF(B6=2,Personality!D3,IF(B6=3,Personality!D4,IF(B6=4,Personality!D5,IF(B6=5,Personality!D6,IF(B6=6,Personality!D7,IF(B6=7,Personality!D8,IF(B6=8,Personality!D9,IF(B6=9,Personality!D10,IF(B6=10,Personality!D11,IF(B6=11,Personality!D12,IF(B6=12,Personality!D13,IF(B6=13,Personality!D14,IF(B6=14,Personality!D15,IF(B6=15,Personality!D16,IF(B6=16,Personality!D17,IF(B6=17,Personality!D18,IF(B6=18,Personality!D19,IF(B6=19,Personality!D20,IF(B6=20,Personality!D21,IF(B6=21,Personality!D22,IF(B6=22,Personality!D23,IF(B6=23,Personality!D24,IF(B6=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
         <f>IF(B6=1,Personality!E2,IF(B6=2,Personality!E3,IF(B6=3,Personality!E4,IF(B6=4,Personality!E5,IF(B6=5,Personality!E6,IF(B6=6,Personality!E7,IF(B6=7,Personality!E8,IF(B6=8,Personality!E9,IF(B6=9,Personality!E10,IF(B6=10,Personality!E11,IF(B6=11,Personality!E12,IF(B6=12,Personality!E13,IF(B6=13,Personality!E14,IF(B6=14,Personality!E15,IF(B6=15,Personality!E16,IF(B6=16,Personality!E17,IF(B6=17,Personality!E18,IF(B6=18,Personality!E19,IF(B6=19,Personality!E20,IF(B6=20,Personality!E21,IF(B6=21,Personality!E22,IF(B6=22,Personality!E23,IF(B6=23,Personality!E24,IF(B6=24,Personality!E25,""))))))))))))))))))))))))</f>
@@ -1101,7 +1164,7 @@
       </c>
       <c r="G6" s="2">
         <f>IF(B6=1,Personality!F2,IF(B6=2,Personality!F3,IF(B6=3,Personality!F4,IF(B6=4,Personality!F5,IF(B6=5,Personality!F6,IF(B6=6,Personality!F7,IF(B6=7,Personality!F8,IF(B6=8,Personality!F9,IF(B6=9,Personality!F10,IF(B6=10,Personality!F11,IF(B6=11,Personality!F12,IF(B6=12,Personality!F13,IF(B6=13,Personality!F14,IF(B6=14,Personality!F15,IF(B6=15,Personality!F16,IF(B6=16,Personality!F17,IF(B6=17,Personality!F18,IF(B6=18,Personality!F19,IF(B6=19,Personality!F20,IF(B6=20,Personality!F21,IF(B6=21,Personality!F22,IF(B6=22,Personality!F23,IF(B6=23,Personality!F24,IF(B6=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -1147,7 +1210,7 @@
     <row r="8" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
         <f>IF(B8=1,Personality!I2,IF(B8=2,Personality!I3,IF(B8=3,Personality!I4,IF(B8=4,Personality!I5,IF(B8=5,Personality!I6,IF(B8=6,Personality!I7,IF(B8=7,Personality!I8,IF(B8=8,Personality!I9,IF(B8=9,Personality!I10,IF(B8=10,Personality!I11,IF(B8=11,Personality!I12,IF(B8=12,Personality!I13,IF(B8=13,Personality!I14,IF(B8=14,Personality!I15,IF(B8=15,Personality!I16,IF(B8=16,Personality!I17,IF(B8=17,Personality!I18,IF(B8=18,Personality!I19,IF(B8=19,Personality!I20,IF(B8=20,Personality!I21,IF(B8=21,Personality!I22,IF(B8=22,Personality!I23,IF(B8=23,Personality!I24,IF(B8=24,Personality!I25,IF(B8=25,Personality!I26,"")))))))))))))))))))))))))</f>
@@ -1155,7 +1218,7 @@
       </c>
       <c r="E8" s="2">
         <f>IF(B8=1,Personality!J2,IF(B8=2,Personality!J3,IF(B8=3,Personality!J4,IF(B8=4,Personality!J5,IF(B8=5,Personality!J6,IF(B8=6,Personality!J7,IF(B8=7,Personality!J8,IF(B8=8,Personality!J9,IF(B8=9,Personality!J10,IF(B8=10,Personality!J11,IF(B8=11,Personality!J12,IF(B8=12,Personality!J13,IF(B8=13,Personality!J14,IF(B8=14,Personality!J15,IF(B8=15,Personality!J16,IF(B8=16,Personality!J17,IF(B8=17,Personality!J18,IF(B8=18,Personality!J19,IF(B8=19,Personality!J20,IF(B8=20,Personality!J21,IF(B8=21,Personality!J22,IF(B8=22,Personality!J23,IF(B8=23,Personality!J24,IF(B8=24,Personality!J25,IF(B8=25,Personality!J26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
         <f>IF(B8=1,Personality!K2,IF(B8=2,Personality!K3,IF(B8=3,Personality!K4,IF(B8=4,Personality!K5,IF(B8=5,Personality!K6,IF(B8=6,Personality!K7,IF(B8=7,Personality!K8,IF(B8=8,Personality!K9,IF(B8=9,Personality!K10,IF(B8=10,Personality!K11,IF(B8=11,Personality!K12,IF(B8=12,Personality!K13,IF(B8=13,Personality!K14,IF(B8=14,Personality!K15,IF(B8=15,Personality!K16,IF(B8=16,Personality!K17,IF(B8=17,Personality!K18,IF(B8=18,Personality!K19,IF(B8=19,Personality!K20,IF(B8=20,Personality!K21,IF(B8=21,Personality!K22,IF(B8=22,Personality!K23,IF(B8=23,Personality!K24,IF(B8=24,Personality!K25,IF(B8=25,Personality!K26,"")))))))))))))))))))))))))</f>
@@ -1247,13 +1310,9 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="B11" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -1272,9 +1331,27 @@
       <c r="X11" s="17"/>
       <c r="Y11" s="17"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <f>IF(B12=1,Personality!I2,IF(B12=2,Personality!I3,IF(B12=3,Personality!I4,IF(B12=4,Personality!I5,IF(B12=5,Personality!I6,IF(B12=6,Personality!I7,IF(B12=7,Personality!I8,IF(B12=8,Personality!I9,IF(B12=9,Personality!I10,IF(B12=10,Personality!I11,IF(B12=11,Personality!I12,IF(B12=12,Personality!I13,IF(B12=13,Personality!I14,IF(B12=14,Personality!I15,IF(B12=15,Personality!I16,IF(B12=16,Personality!I17,IF(B12=17,Personality!I18,IF(B12=18,Personality!I19,IF(B12=19,Personality!I20,IF(B12=20,Personality!I21,IF(B12=21,Personality!I22,IF(B12=22,Personality!I23,IF(B12=23,Personality!I24,IF(B12=24,Personality!I25,IF(B12=25,Personality!I26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <f>IF(B12=1,Personality!J2,IF(B12=2,Personality!J3,IF(B12=3,Personality!J4,IF(B12=4,Personality!J5,IF(B12=5,Personality!J6,IF(B12=6,Personality!J7,IF(B12=7,Personality!J8,IF(B12=8,Personality!J9,IF(B12=9,Personality!J10,IF(B12=10,Personality!J11,IF(B12=11,Personality!J12,IF(B12=12,Personality!J13,IF(B12=13,Personality!J14,IF(B12=14,Personality!J15,IF(B12=15,Personality!J16,IF(B12=16,Personality!J17,IF(B12=17,Personality!J18,IF(B12=18,Personality!J19,IF(B12=19,Personality!J20,IF(B12=20,Personality!J21,IF(B12=21,Personality!J22,IF(B12=22,Personality!J23,IF(B12=23,Personality!J24,IF(B12=24,Personality!J25,IF(B12=25,Personality!J26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f>IF(B12=1,Personality!K2,IF(B12=2,Personality!K3,IF(B12=3,Personality!K4,IF(B12=4,Personality!K5,IF(B12=5,Personality!K6,IF(B12=6,Personality!K7,IF(B12=7,Personality!K8,IF(B12=8,Personality!K9,IF(B12=9,Personality!K10,IF(B12=10,Personality!K11,IF(B12=11,Personality!K12,IF(B12=12,Personality!K13,IF(B12=13,Personality!K14,IF(B12=14,Personality!K15,IF(B12=15,Personality!K16,IF(B12=16,Personality!K17,IF(B12=17,Personality!K18,IF(B12=18,Personality!K19,IF(B12=19,Personality!K20,IF(B12=20,Personality!K21,IF(B12=21,Personality!K22,IF(B12=22,Personality!K23,IF(B12=23,Personality!K24,IF(B12=24,Personality!K25,IF(B12=25,Personality!K26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f>IF(B12=1,Personality!L2,IF(B12=2,Personality!L3,IF(B12=3,Personality!L4,IF(B12=4,Personality!L5,IF(B12=5,Personality!L6,IF(B12=6,Personality!L7,IF(B12=7,Personality!L8,IF(B12=8,Personality!L9,IF(B12=9,Personality!L10,IF(B12=10,Personality!L11,IF(B12=11,Personality!L12,IF(B12=12,Personality!L13,IF(B12=13,Personality!L14,IF(B12=14,Personality!L15,IF(B12=15,Personality!L16,IF(B12=16,Personality!L17,IF(B12=17,Personality!L18,IF(B12=18,Personality!L19,IF(B12=19,Personality!L20,IF(B12=20,Personality!L21,IF(B12=21,Personality!L22,IF(B12=22,Personality!L23,IF(B12=23,Personality!L24,IF(B12=24,Personality!L25,IF(B12=25,Personality!L26,"")))))))))))))))))))))))))</f>
+        <v>0</v>
+      </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -1293,28 +1370,15 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="14"/>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3">
-        <f>D4+D6+D8+D10</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" ref="E13:G13" si="0">E4+E6+E8+E10</f>
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
@@ -1333,21 +1397,9 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
     </row>
-    <row r="14" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="14"/>
-      <c r="D14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>10</v>
-      </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
@@ -1366,27 +1418,27 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="17"/>
     </row>
-    <row r="15" spans="1:25" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="7">
-        <f>IF(D13=0,1,D13)</f>
-        <v>3</v>
-      </c>
-      <c r="E15" s="8">
-        <f>IF(E13=0,1,E13)</f>
-        <v>3</v>
-      </c>
-      <c r="F15" s="8">
-        <f>IF(F13=0,1,F13)</f>
-        <v>5</v>
-      </c>
-      <c r="G15" s="9">
-        <f>IF(G13=0,1,G13)</f>
-        <v>3</v>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3">
+        <f>D4+D6+D8+D10+D12</f>
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" ref="E15:G15" si="0">E4+E6+E8+E10+E12</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -1406,9 +1458,21 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="17"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="14"/>
+      <c r="D16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
@@ -1427,15 +1491,28 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="17"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7">
+        <f>IF(D15=0,1,D15)</f>
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <f>IF(E15=0,1,E15)</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <f>IF(F15=0,1,F15)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="9">
+        <f>IF(G15=0,1,G15)</f>
+        <v>1</v>
+      </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
@@ -1456,13 +1533,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="14"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
@@ -1669,6 +1740,60 @@
       <c r="W25" s="17"/>
       <c r="X25" s="17"/>
       <c r="Y25" s="17"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,6 +1891,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1037" r:id="rId8" name="Drop Down 13">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1581150</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>400050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>

<commit_message>
Localisation merged Fixed JAP and stability_war_support decisions by Lordlemos Several country traits reworked by vprozevski Svevral countryfiles reworked Fixed missing gfx in leadergroups.gui Renamed national-equipment with tag as last
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="0" windowWidth="18180" windowHeight="8085"/>
+    <workbookView xWindow="10500" yWindow="0" windowWidth="18180" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Skill level" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$B$2:$H$18</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcCompleted="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -377,15 +378,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="4" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="22" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="18" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="7" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -632,14 +633,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="1504950" cy="361950"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1581150</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>400050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Drop Down 12" hidden="1">
@@ -648,7 +654,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CAEA6A3-B0FE-4734-AE4B-730501C5812B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -679,7 +685,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -987,7 +993,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,15 +1091,15 @@
     <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
         <f>IF(B4=1,Skills!C2,IF(B4=2,Skills!C3,IF(B4=3,Skills!C4,IF(B4=4,Skills!C5,IF(B4=5,Skills!C6,IF(B4=6,Skills!C7,IF(B4=7,Skills!C8,IF(B4=8,Skills!C9,IF(B4=9,Skills!C10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <f>IF(B4=1,Skills!D2,IF(B4=2,Skills!D3,IF(B4=3,Skills!D4,IF(B4=4,Skills!D5,IF(B4=5,Skills!D6,IF(B4=6,Skills!D7,IF(B4=7,Skills!D8,IF(B4=8,Skills!D9,IF(B4=9,Skills!D10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
         <f>IF(B4=1,Skills!E2,IF(B4=2,Skills!E3,IF(B4=3,Skills!E4,IF(B4=4,Skills!E5,IF(B4=5,Skills!E6,IF(B4=6,Skills!E7,IF(B4=7,Skills!E8,IF(B4=8,Skills!E9,IF(B4=9,Skills!E10,"")))))))))</f>
@@ -1101,7 +1107,7 @@
       </c>
       <c r="G4" s="2">
         <f>IF(B4=1,Skills!F2,IF(B4=2,Skills!F3,IF(B4=3,Skills!F4,IF(B4=4,Skills!F5,IF(B4=5,Skills!F6,IF(B4=6,Skills!F7,IF(B4=7,Skills!F8,IF(B4=8,Skills!F9,IF(B4=9,Skills!F10,"")))))))))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -1147,24 +1153,24 @@
     <row r="6" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
         <f>IF(B6=1,Personality!C2,IF(B6=2,Personality!C3,IF(B6=3,Personality!C4,IF(B6=4,Personality!C5,IF(B6=5,Personality!C6,IF(B6=6,Personality!C7,IF(B6=7,Personality!C8,IF(B6=8,Personality!C9,IF(B6=9,Personality!C10,IF(B6=10,Personality!C11,IF(B6=11,Personality!C12,IF(B6=12,Personality!C13,IF(B6=13,Personality!C14,IF(B6=14,Personality!C15,IF(B6=15,Personality!C16,IF(B6=16,Personality!C17,IF(B6=17,Personality!C18,IF(B6=18,Personality!C19,IF(B6=19,Personality!C20,IF(B6=20,Personality!C21,IF(B6=21,Personality!C22,IF(B6=22,Personality!C23,IF(B6=23,Personality!C24,IF(B6=24,Personality!C25,""))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E6" s="2">
         <f>IF(B6=1,Personality!D2,IF(B6=2,Personality!D3,IF(B6=3,Personality!D4,IF(B6=4,Personality!D5,IF(B6=5,Personality!D6,IF(B6=6,Personality!D7,IF(B6=7,Personality!D8,IF(B6=8,Personality!D9,IF(B6=9,Personality!D10,IF(B6=10,Personality!D11,IF(B6=11,Personality!D12,IF(B6=12,Personality!D13,IF(B6=13,Personality!D14,IF(B6=14,Personality!D15,IF(B6=15,Personality!D16,IF(B6=16,Personality!D17,IF(B6=17,Personality!D18,IF(B6=18,Personality!D19,IF(B6=19,Personality!D20,IF(B6=20,Personality!D21,IF(B6=21,Personality!D22,IF(B6=22,Personality!D23,IF(B6=23,Personality!D24,IF(B6=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6" s="2">
         <f>IF(B6=1,Personality!E2,IF(B6=2,Personality!E3,IF(B6=3,Personality!E4,IF(B6=4,Personality!E5,IF(B6=5,Personality!E6,IF(B6=6,Personality!E7,IF(B6=7,Personality!E8,IF(B6=8,Personality!E9,IF(B6=9,Personality!E10,IF(B6=10,Personality!E11,IF(B6=11,Personality!E12,IF(B6=12,Personality!E13,IF(B6=13,Personality!E14,IF(B6=14,Personality!E15,IF(B6=15,Personality!E16,IF(B6=16,Personality!E17,IF(B6=17,Personality!E18,IF(B6=18,Personality!E19,IF(B6=19,Personality!E20,IF(B6=20,Personality!E21,IF(B6=21,Personality!E22,IF(B6=22,Personality!E23,IF(B6=23,Personality!E24,IF(B6=24,Personality!E25,""))))))))))))))))))))))))</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="G6" s="2">
         <f>IF(B6=1,Personality!F2,IF(B6=2,Personality!F3,IF(B6=3,Personality!F4,IF(B6=4,Personality!F5,IF(B6=5,Personality!F6,IF(B6=6,Personality!F7,IF(B6=7,Personality!F8,IF(B6=8,Personality!F9,IF(B6=9,Personality!F10,IF(B6=10,Personality!F11,IF(B6=11,Personality!F12,IF(B6=12,Personality!F13,IF(B6=13,Personality!F14,IF(B6=14,Personality!F15,IF(B6=15,Personality!F16,IF(B6=16,Personality!F17,IF(B6=17,Personality!F18,IF(B6=18,Personality!F19,IF(B6=19,Personality!F20,IF(B6=20,Personality!F21,IF(B6=21,Personality!F22,IF(B6=22,Personality!F23,IF(B6=23,Personality!F24,IF(B6=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -1210,19 +1216,19 @@
     <row r="8" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2">
         <f>IF(B8=1,Personality!I2,IF(B8=2,Personality!I3,IF(B8=3,Personality!I4,IF(B8=4,Personality!I5,IF(B8=5,Personality!I6,IF(B8=6,Personality!I7,IF(B8=7,Personality!I8,IF(B8=8,Personality!I9,IF(B8=9,Personality!I10,IF(B8=10,Personality!I11,IF(B8=11,Personality!I12,IF(B8=12,Personality!I13,IF(B8=13,Personality!I14,IF(B8=14,Personality!I15,IF(B8=15,Personality!I16,IF(B8=16,Personality!I17,IF(B8=17,Personality!I18,IF(B8=18,Personality!I19,IF(B8=19,Personality!I20,IF(B8=20,Personality!I21,IF(B8=21,Personality!I22,IF(B8=22,Personality!I23,IF(B8=23,Personality!I24,IF(B8=24,Personality!I25,IF(B8=25,Personality!I26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E8" s="2">
         <f>IF(B8=1,Personality!J2,IF(B8=2,Personality!J3,IF(B8=3,Personality!J4,IF(B8=4,Personality!J5,IF(B8=5,Personality!J6,IF(B8=6,Personality!J7,IF(B8=7,Personality!J8,IF(B8=8,Personality!J9,IF(B8=9,Personality!J10,IF(B8=10,Personality!J11,IF(B8=11,Personality!J12,IF(B8=12,Personality!J13,IF(B8=13,Personality!J14,IF(B8=14,Personality!J15,IF(B8=15,Personality!J16,IF(B8=16,Personality!J17,IF(B8=17,Personality!J18,IF(B8=18,Personality!J19,IF(B8=19,Personality!J20,IF(B8=20,Personality!J21,IF(B8=21,Personality!J22,IF(B8=22,Personality!J23,IF(B8=23,Personality!J24,IF(B8=24,Personality!J25,IF(B8=25,Personality!J26,"")))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F8" s="2">
         <f>IF(B8=1,Personality!K2,IF(B8=2,Personality!K3,IF(B8=3,Personality!K4,IF(B8=4,Personality!K5,IF(B8=5,Personality!K6,IF(B8=6,Personality!K7,IF(B8=7,Personality!K8,IF(B8=8,Personality!K9,IF(B8=9,Personality!K10,IF(B8=10,Personality!K11,IF(B8=11,Personality!K12,IF(B8=12,Personality!K13,IF(B8=13,Personality!K14,IF(B8=14,Personality!K15,IF(B8=15,Personality!K16,IF(B8=16,Personality!K17,IF(B8=17,Personality!K18,IF(B8=18,Personality!K19,IF(B8=19,Personality!K20,IF(B8=20,Personality!K21,IF(B8=21,Personality!K22,IF(B8=22,Personality!K23,IF(B8=23,Personality!K24,IF(B8=24,Personality!K25,IF(B8=25,Personality!K26,"")))))))))))))))))))))))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2">
         <f>IF(B8=1,Personality!L2,IF(B8=2,Personality!L3,IF(B8=3,Personality!L4,IF(B8=4,Personality!L5,IF(B8=5,Personality!L6,IF(B8=6,Personality!L7,IF(B8=7,Personality!L8,IF(B8=8,Personality!L9,IF(B8=9,Personality!L10,IF(B8=10,Personality!L11,IF(B8=11,Personality!L12,IF(B8=12,Personality!L13,IF(B8=13,Personality!L14,IF(B8=14,Personality!L15,IF(B8=15,Personality!L16,IF(B8=16,Personality!L17,IF(B8=17,Personality!L18,IF(B8=18,Personality!L19,IF(B8=19,Personality!L20,IF(B8=20,Personality!L21,IF(B8=21,Personality!L22,IF(B8=22,Personality!L23,IF(B8=23,Personality!L24,IF(B8=24,Personality!L25,IF(B8=25,Personality!L26,"")))))))))))))))))))))))))</f>
@@ -1426,18 +1432,18 @@
       </c>
       <c r="D15" s="3">
         <f>D4+D6+D8+D10+D12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ref="E15:G15" si="0">E4+E6+E8+E10+E12</f>
-        <v>2</v>
+        <f>E4+E6+E8+E10+E12</f>
+        <v>0</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>F4+F6+F8+F10+F12</f>
+        <v>0</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f>G4+G6+G8+G10+G12</f>
         <v>1</v>
       </c>
       <c r="I15" s="17"/>
@@ -1499,15 +1505,15 @@
       </c>
       <c r="D17" s="7">
         <f>IF(D15=0,1,D15)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8">
         <f>IF(E15=0,1,E15)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="8">
         <f>IF(F15=0,1,F15)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G17" s="9">
         <f>IF(G15=0,1,G15)</f>

</xml_diff>

<commit_message>
Several typos all over the board Added decisions for Motorise the 29. Inf-Div and forming the 4. Leichte Division. CC and FM no modifiers Added divisiongroup_names to several GER units
</commit_message>
<xml_diff>
--- a/BICE modfile/Generals Skill levels.xlsx
+++ b/BICE modfile/Generals Skill levels.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\maver\Documents\Paradox Interactive\Hearts of Iron IV\mod\Blackice-WIP-v2.5\BICE modfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2D95B68D-A871-4360-AC21-35A464294F05}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="0" windowWidth="18180" windowHeight="8085"/>
+    <workbookView xWindow="10500" yWindow="0" windowWidth="18180" windowHeight="8085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skill level" sheetId="3" r:id="rId1"/>
@@ -19,8 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Skill level'!$B$2:$H$18</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcCompleted="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,15 +378,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="4" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="10" dropStyle="combo" dx="22" fmlaLink="'Skill level'!$B$4" fmlaRange="Skills!$A$2:$A$10" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="18" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$8" fmlaRange="Personality!$H$2:$H$26" sel="22" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="5" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="25" dropStyle="combo" dx="22" fmlaLink="$B$6" fmlaRange="Personality!$B$2:$B$25" sel="6" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -988,7 +988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:Y27"/>
   <sheetViews>
@@ -1091,15 +1091,15 @@
     <row r="4" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
         <f>IF(B4=1,Skills!C2,IF(B4=2,Skills!C3,IF(B4=3,Skills!C4,IF(B4=4,Skills!C5,IF(B4=5,Skills!C6,IF(B4=6,Skills!C7,IF(B4=7,Skills!C8,IF(B4=8,Skills!C9,IF(B4=9,Skills!C10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <f>IF(B4=1,Skills!D2,IF(B4=2,Skills!D3,IF(B4=3,Skills!D4,IF(B4=4,Skills!D5,IF(B4=5,Skills!D6,IF(B4=6,Skills!D7,IF(B4=7,Skills!D8,IF(B4=8,Skills!D9,IF(B4=9,Skills!D10,"")))))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
         <f>IF(B4=1,Skills!E2,IF(B4=2,Skills!E3,IF(B4=3,Skills!E4,IF(B4=4,Skills!E5,IF(B4=5,Skills!E6,IF(B4=6,Skills!E7,IF(B4=7,Skills!E8,IF(B4=8,Skills!E9,IF(B4=9,Skills!E10,"")))))))))</f>
@@ -1153,24 +1153,24 @@
     <row r="6" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
         <f>IF(B6=1,Personality!C2,IF(B6=2,Personality!C3,IF(B6=3,Personality!C4,IF(B6=4,Personality!C5,IF(B6=5,Personality!C6,IF(B6=6,Personality!C7,IF(B6=7,Personality!C8,IF(B6=8,Personality!C9,IF(B6=9,Personality!C10,IF(B6=10,Personality!C11,IF(B6=11,Personality!C12,IF(B6=12,Personality!C13,IF(B6=13,Personality!C14,IF(B6=14,Personality!C15,IF(B6=15,Personality!C16,IF(B6=16,Personality!C17,IF(B6=17,Personality!C18,IF(B6=18,Personality!C19,IF(B6=19,Personality!C20,IF(B6=20,Personality!C21,IF(B6=21,Personality!C22,IF(B6=22,Personality!C23,IF(B6=23,Personality!C24,IF(B6=24,Personality!C25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <f>IF(B6=1,Personality!D2,IF(B6=2,Personality!D3,IF(B6=3,Personality!D4,IF(B6=4,Personality!D5,IF(B6=5,Personality!D6,IF(B6=6,Personality!D7,IF(B6=7,Personality!D8,IF(B6=8,Personality!D9,IF(B6=9,Personality!D10,IF(B6=10,Personality!D11,IF(B6=11,Personality!D12,IF(B6=12,Personality!D13,IF(B6=13,Personality!D14,IF(B6=14,Personality!D15,IF(B6=15,Personality!D16,IF(B6=16,Personality!D17,IF(B6=17,Personality!D18,IF(B6=18,Personality!D19,IF(B6=19,Personality!D20,IF(B6=20,Personality!D21,IF(B6=21,Personality!D22,IF(B6=22,Personality!D23,IF(B6=23,Personality!D24,IF(B6=24,Personality!D25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
         <f>IF(B6=1,Personality!E2,IF(B6=2,Personality!E3,IF(B6=3,Personality!E4,IF(B6=4,Personality!E5,IF(B6=5,Personality!E6,IF(B6=6,Personality!E7,IF(B6=7,Personality!E8,IF(B6=8,Personality!E9,IF(B6=9,Personality!E10,IF(B6=10,Personality!E11,IF(B6=11,Personality!E12,IF(B6=12,Personality!E13,IF(B6=13,Personality!E14,IF(B6=14,Personality!E15,IF(B6=15,Personality!E16,IF(B6=16,Personality!E17,IF(B6=17,Personality!E18,IF(B6=18,Personality!E19,IF(B6=19,Personality!E20,IF(B6=20,Personality!E21,IF(B6=21,Personality!E22,IF(B6=22,Personality!E23,IF(B6=23,Personality!E24,IF(B6=24,Personality!E25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <f>IF(B6=1,Personality!F2,IF(B6=2,Personality!F3,IF(B6=3,Personality!F4,IF(B6=4,Personality!F5,IF(B6=5,Personality!F6,IF(B6=6,Personality!F7,IF(B6=7,Personality!F8,IF(B6=8,Personality!F9,IF(B6=9,Personality!F10,IF(B6=10,Personality!F11,IF(B6=11,Personality!F12,IF(B6=12,Personality!F13,IF(B6=13,Personality!F14,IF(B6=14,Personality!F15,IF(B6=15,Personality!F16,IF(B6=16,Personality!F17,IF(B6=17,Personality!F18,IF(B6=18,Personality!F19,IF(B6=19,Personality!F20,IF(B6=20,Personality!F21,IF(B6=21,Personality!F22,IF(B6=22,Personality!F23,IF(B6=23,Personality!F24,IF(B6=24,Personality!F25,""))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -1216,19 +1216,19 @@
     <row r="8" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
         <f>IF(B8=1,Personality!I2,IF(B8=2,Personality!I3,IF(B8=3,Personality!I4,IF(B8=4,Personality!I5,IF(B8=5,Personality!I6,IF(B8=6,Personality!I7,IF(B8=7,Personality!I8,IF(B8=8,Personality!I9,IF(B8=9,Personality!I10,IF(B8=10,Personality!I11,IF(B8=11,Personality!I12,IF(B8=12,Personality!I13,IF(B8=13,Personality!I14,IF(B8=14,Personality!I15,IF(B8=15,Personality!I16,IF(B8=16,Personality!I17,IF(B8=17,Personality!I18,IF(B8=18,Personality!I19,IF(B8=19,Personality!I20,IF(B8=20,Personality!I21,IF(B8=21,Personality!I22,IF(B8=22,Personality!I23,IF(B8=23,Personality!I24,IF(B8=24,Personality!I25,IF(B8=25,Personality!I26,"")))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <f>IF(B8=1,Personality!J2,IF(B8=2,Personality!J3,IF(B8=3,Personality!J4,IF(B8=4,Personality!J5,IF(B8=5,Personality!J6,IF(B8=6,Personality!J7,IF(B8=7,Personality!J8,IF(B8=8,Personality!J9,IF(B8=9,Personality!J10,IF(B8=10,Personality!J11,IF(B8=11,Personality!J12,IF(B8=12,Personality!J13,IF(B8=13,Personality!J14,IF(B8=14,Personality!J15,IF(B8=15,Personality!J16,IF(B8=16,Personality!J17,IF(B8=17,Personality!J18,IF(B8=18,Personality!J19,IF(B8=19,Personality!J20,IF(B8=20,Personality!J21,IF(B8=21,Personality!J22,IF(B8=22,Personality!J23,IF(B8=23,Personality!J24,IF(B8=24,Personality!J25,IF(B8=25,Personality!J26,"")))))))))))))))))))))))))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
         <f>IF(B8=1,Personality!K2,IF(B8=2,Personality!K3,IF(B8=3,Personality!K4,IF(B8=4,Personality!K5,IF(B8=5,Personality!K6,IF(B8=6,Personality!K7,IF(B8=7,Personality!K8,IF(B8=8,Personality!K9,IF(B8=9,Personality!K10,IF(B8=10,Personality!K11,IF(B8=11,Personality!K12,IF(B8=12,Personality!K13,IF(B8=13,Personality!K14,IF(B8=14,Personality!K15,IF(B8=15,Personality!K16,IF(B8=16,Personality!K17,IF(B8=17,Personality!K18,IF(B8=18,Personality!K19,IF(B8=19,Personality!K20,IF(B8=20,Personality!K21,IF(B8=21,Personality!K22,IF(B8=22,Personality!K23,IF(B8=23,Personality!K24,IF(B8=24,Personality!K25,IF(B8=25,Personality!K26,"")))))))))))))))))))))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
         <f>IF(B8=1,Personality!L2,IF(B8=2,Personality!L3,IF(B8=3,Personality!L4,IF(B8=4,Personality!L5,IF(B8=5,Personality!L6,IF(B8=6,Personality!L7,IF(B8=7,Personality!L8,IF(B8=8,Personality!L9,IF(B8=9,Personality!L10,IF(B8=10,Personality!L11,IF(B8=11,Personality!L12,IF(B8=12,Personality!L13,IF(B8=13,Personality!L14,IF(B8=14,Personality!L15,IF(B8=15,Personality!L16,IF(B8=16,Personality!L17,IF(B8=17,Personality!L18,IF(B8=18,Personality!L19,IF(B8=19,Personality!L20,IF(B8=20,Personality!L21,IF(B8=21,Personality!L22,IF(B8=22,Personality!L23,IF(B8=23,Personality!L24,IF(B8=24,Personality!L25,IF(B8=25,Personality!L26,"")))))))))))))))))))))))))</f>
@@ -1432,19 +1432,19 @@
       </c>
       <c r="D15" s="3">
         <f>D4+D6+D8+D10+D12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
         <f>E4+E6+E8+E10+E12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="3">
         <f>F4+F6+F8+F10+F12</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G15" s="3">
         <f>G4+G6+G8+G10+G12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -1505,19 +1505,19 @@
       </c>
       <c r="D17" s="7">
         <f>IF(D15=0,1,D15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="8">
         <f>IF(E15=0,1,E15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="8">
         <f>IF(F15=0,1,F15)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17" s="9">
         <f>IF(G15=0,1,G15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -1926,7 +1926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N10"/>
   <sheetViews>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:L26"/>
   <sheetViews>

</xml_diff>